<commit_message>
Unrestricted datapipeline updated - need source change or update
</commit_message>
<xml_diff>
--- a/DataSources.xlsx
+++ b/DataSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B606801-9E67-4853-8804-1DEBBA2F2FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63132AFF-8B2E-4242-B619-C2EFEE754570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="2440" windowWidth="24220" windowHeight="13120" xr2:uid="{3EF8ABA0-F62A-49A4-AC27-CE9CB6EB98F7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3EF8ABA0-F62A-49A4-AC27-CE9CB6EB98F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>API</t>
   </si>
@@ -183,34 +183,28 @@
     <t>#</t>
   </si>
   <si>
-    <t>fert_actual</t>
-  </si>
-  <si>
-    <t>fert_forecast</t>
-  </si>
-  <si>
-    <t>fpi_actual</t>
-  </si>
-  <si>
-    <t>fpi_forecast</t>
-  </si>
-  <si>
-    <t>gdp_actual</t>
-  </si>
-  <si>
-    <t>gdp_forecast</t>
-  </si>
-  <si>
-    <t>ng_actual</t>
-  </si>
-  <si>
-    <t>ng_forecast</t>
-  </si>
-  <si>
-    <t>usdeur_actual</t>
-  </si>
-  <si>
-    <t>usdeur_forecast</t>
+    <t>FERT</t>
+  </si>
+  <si>
+    <t>FPI</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>USDEUR</t>
+  </si>
+  <si>
+    <t>INTERVAL</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -415,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -479,29 +473,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -819,6 +796,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -833,12 +826,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -855,19 +850,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86475FD9-E9E3-4407-BDB4-0A3EC12F66E9}" name="Table2" displayName="Table2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86475FD9-E9E3-4407-BDB4-0A3EC12F66E9}" name="Table2" displayName="Table2" ref="A1:I11" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
     <sortCondition ref="C1:C11"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C7D83ED6-755F-4306-A457-3F6CED970860}" name="#" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1BF275A4-9464-4885-9268-7F212BED4A70}" name="API" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{BEEAE549-2CD3-42E1-BE72-00BD465229BD}" name="SRC" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D3972C66-1249-4CEB-AC91-61DC21C7A190}" name="TYPE" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{E24DC55F-F11A-403B-9C4F-35415C7F2BA4}" name="Download type" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{9414E5DF-A2E5-4BB1-90F4-8390B2E10B67}" name="STATUS" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9DDBCE86-4D09-4D93-B33D-6515315E03D7}" name="S3 Location" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{12DE8A9E-D5BF-4C92-BCFF-0F95686BFAF7}" name="Frequency of Run" dataDxfId="1"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{C7D83ED6-755F-4306-A457-3F6CED970860}" name="#" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1BF275A4-9464-4885-9268-7F212BED4A70}" name="API" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{BEEAE549-2CD3-42E1-BE72-00BD465229BD}" name="SRC" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D3972C66-1249-4CEB-AC91-61DC21C7A190}" name="TYPE" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E24DC55F-F11A-403B-9C4F-35415C7F2BA4}" name="Download type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9414E5DF-A2E5-4BB1-90F4-8390B2E10B67}" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{9DDBCE86-4D09-4D93-B33D-6515315E03D7}" name="S3 Location" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{12DE8A9E-D5BF-4C92-BCFF-0F95686BFAF7}" name="Frequency of Run" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{3CC4B135-9275-4957-B984-AC4A6507195C}" name="INTERVAL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1170,17 +1166,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9690B94-8EE9-4E17-964D-48FC3B30410C}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="7.1796875" customWidth="1"/>
     <col min="5" max="5" width="34.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.90625" customWidth="1"/>
@@ -1188,7 +1184,7 @@
     <col min="8" max="8" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1213,8 +1209,11 @@
       <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="I1" s="23" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
@@ -1239,8 +1238,11 @@
       <c r="H2" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
@@ -1248,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>23</v>
@@ -1265,8 +1267,11 @@
       <c r="H3" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>22</v>
@@ -1291,8 +1296,11 @@
       <c r="H4" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>46</v>
       </c>
@@ -1300,7 +1308,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>23</v>
@@ -1318,7 +1326,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1326,7 +1334,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -1343,8 +1351,11 @@
       <c r="H6" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
@@ -1352,7 +1363,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>23</v>
@@ -1369,8 +1380,11 @@
       <c r="H7" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1392,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>22</v>
@@ -1395,8 +1409,11 @@
       <c r="H8" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1404,7 +1421,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>23</v>
@@ -1421,8 +1438,11 @@
       <c r="H9" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1430,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>22</v>
@@ -1447,8 +1467,11 @@
       <c r="H10" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>37</v>
       </c>
@@ -1456,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>23</v>
@@ -1473,8 +1496,11 @@
       <c r="H11" s="19" t="s">
         <v>39</v>
       </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
AWS Restricted link added
</commit_message>
<xml_diff>
--- a/DataSources.xlsx
+++ b/DataSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63132AFF-8B2E-4242-B619-C2EFEE754570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D140FA1D-2394-46A3-A171-6C4B3DFACF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3EF8ABA0-F62A-49A4-AC27-CE9CB6EB98F7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{3EF8ABA0-F62A-49A4-AC27-CE9CB6EB98F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>API</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>s3://insights-shared-prod-data-lake-non-hr/CLEANED/EXTERNAL/system=fao/usecase=FoodPriceIndexForecast/FoodPriceIndex-forecast.parquet</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9690B94-8EE9-4E17-964D-48FC3B30410C}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1320,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>39</v>

</xml_diff>